<commit_message>
subida inicial del comparativo
</commit_message>
<xml_diff>
--- a/tblInfFlujoCaja_Proyección_Agosto_2025_Junio_2026.xlsx
+++ b/tblInfFlujoCaja_Proyección_Agosto_2025_Junio_2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\manager8\comunes\importacion\api_cluster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7B7BA9-63E0-4D3E-A080-D51AAB398C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280B2A70-EFF6-41F9-9254-BD4E4E4F71F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -978,9 +978,6 @@
     <t>Gastos y comisiones Bancarias ( BANCO CHILE - SECURITY )</t>
   </si>
   <si>
-    <t>2.01.07.01 - Proveedores Arrdo  Oficina , estacionamiento ,Kame</t>
-  </si>
-  <si>
     <t xml:space="preserve">PROVEEDORES VARIABLE </t>
   </si>
   <si>
@@ -1009,6 +1006,9 @@
   </si>
   <si>
     <t xml:space="preserve">Compras Brutas Estimadas </t>
+  </si>
+  <si>
+    <t>2.01.07.01 - Proveedores Arrdo  Oficina , estacionamiento</t>
   </si>
 </sst>
 </file>
@@ -2223,7 +2223,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="B14" s="2">
         <f>885000+730000</f>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3257,6 +3257,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11473,7 +11474,7 @@
     </row>
     <row r="80" spans="1:17">
       <c r="N80" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O80" s="3" t="s">
         <v>267</v>
@@ -11482,7 +11483,7 @@
         <v>17636200</v>
       </c>
       <c r="Q80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="81" spans="14:18">
@@ -11490,7 +11491,7 @@
     </row>
     <row r="82" spans="14:18">
       <c r="N82" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P82" s="49">
         <v>39109861</v>
@@ -11502,7 +11503,7 @@
     </row>
     <row r="84" spans="14:18">
       <c r="N84" s="93" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O84" s="101"/>
       <c r="P84" s="93">
@@ -11513,12 +11514,12 @@
         <v>0.3</v>
       </c>
       <c r="R84" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="86" spans="14:18">
       <c r="N86" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P86" s="92">
         <f>1-P84</f>
@@ -13174,7 +13175,7 @@
     </row>
     <row r="12" spans="1:53">
       <c r="A12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B12" s="49"/>
       <c r="C12" s="11">
@@ -13243,7 +13244,7 @@
     </row>
     <row r="14" spans="1:53">
       <c r="A14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C14" s="11">
         <f>+C12/1.19</f>
@@ -13305,7 +13306,7 @@
     </row>
     <row r="16" spans="1:53">
       <c r="A16" s="87" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C16" s="11">
         <f>+C14*0.19</f>

</xml_diff>